<commit_message>
Thêm bảng công ngày chủ nhật
</commit_message>
<xml_diff>
--- a/static/uploads/mau/hopdong/nt1/duoi_o2/hdnh.xlsx
+++ b/static/uploads/mau/hopdong/nt1/duoi_o2/hdnh.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NS7000~1.THU\AppData\Local\Temp\Rar$DIa8892.23610\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAT\Desktop\code\working\HRM\static\uploads\mau\hopdong\nt1\duoi_o2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF385D1-0491-44B9-A3CA-15E0C6D27355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3E9CAD-FF69-4E34-93CF-38757970558B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,443 +28,443 @@
     <t>CỘNG HÒA XÃ HỘI CHỦ NGHĨA VIỆT NAM</t>
   </si>
   <si>
-    <t>Địa chỉ: Rực Liễn - Thuỷ Sơn - Thuỷ Nguyên - Hải Phòng_x000D_
+    <t>Độc lập - Tự do - Hạnh phúc</t>
+  </si>
+  <si>
+    <t>------------------------</t>
+  </si>
+  <si>
+    <t>Số: LC28D/13282</t>
+  </si>
+  <si>
+    <t>Hải Phòng, ngày 05 tháng 06 năm 2024</t>
+  </si>
+  <si>
+    <t>HỢP ĐỒNG LAO ĐỘNG</t>
+  </si>
+  <si>
+    <t>(Căn cứ vào BLLĐ 45/2019/QH 14 và NĐ 145/2020/NĐ-CP, TT 10/2020/TT-BLĐTBXH )</t>
+  </si>
+  <si>
+    <t>Chúng tôi, một bên là</t>
+  </si>
+  <si>
+    <t>Ông/Bà:</t>
+  </si>
+  <si>
+    <t>VŨ THỊ HIỀN</t>
+  </si>
+  <si>
+    <t>Quốc tịch:</t>
+  </si>
+  <si>
+    <t>VIỆT NAM</t>
+  </si>
+  <si>
+    <t>Chức vụ:</t>
+  </si>
+  <si>
+    <t>Trưởng phòng Hành chính Nhân sự</t>
+  </si>
+  <si>
+    <t>Sinh ngày:</t>
+  </si>
+  <si>
+    <t>05/09/1990           Giới tính: Nữ</t>
+  </si>
+  <si>
+    <t>Địa chỉ thường trú:</t>
+  </si>
+  <si>
+    <t>Quyết Tiến 3, An Thắng, An Lão, Hải Phòng</t>
+  </si>
+  <si>
+    <t>Số CCCD:</t>
+  </si>
+  <si>
+    <t>031190008508</t>
+  </si>
+  <si>
+    <t>Cấp ngày:</t>
+  </si>
+  <si>
+    <t>02/03/2022</t>
+  </si>
+  <si>
+    <t>Nơi cấp:</t>
+  </si>
+  <si>
+    <t>Cục cảnh sát</t>
+  </si>
+  <si>
+    <t>Đại diện cho:</t>
+  </si>
+  <si>
+    <t>Địa chỉ:</t>
+  </si>
+  <si>
+    <t>Điện thoại:</t>
+  </si>
+  <si>
+    <t>02253642408</t>
+  </si>
+  <si>
+    <t>Fax:</t>
+  </si>
+  <si>
+    <t>02253642407</t>
+  </si>
+  <si>
+    <t>Và một bên là:</t>
+  </si>
+  <si>
+    <t>BÙI THỊ HUYỀN</t>
+  </si>
+  <si>
+    <t>VIỆT NAM</t>
+  </si>
+  <si>
+    <t>10/03/1991</t>
+  </si>
+  <si>
+    <t>Giới tính:</t>
+  </si>
+  <si>
+    <t>Nữ</t>
+  </si>
+  <si>
+    <t>Thôn 1, Cao Nhân, Thủy Nguyên, Hải Phòng</t>
+  </si>
+  <si>
+    <t>Số CCCD: 31191003277</t>
+  </si>
+  <si>
+    <t>09/08/2021</t>
+  </si>
+  <si>
+    <t>Thỏa thuận ký kết hợp đồng lao động và cam kết làm đúng những điều khoản sau đây:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ĐIỀU 1: HỢP ĐỒNG VÀ CÔNG VIỆC HỢP ĐỒNG </t>
+  </si>
+  <si>
+    <t>- Thời hạn hợp đồng:</t>
+  </si>
+  <si>
+    <t>Hợp đồng xác định thời hạn 28 ngày</t>
+  </si>
+  <si>
+    <t>Từ ngày 05 tháng 06 năm 2024 đến hết ngày 02 tháng 07 năm 2024</t>
+  </si>
+  <si>
+    <t>+ Các địa điểm khác theo sự phân công của Công ty theo yêu cầu công việc</t>
+  </si>
+  <si>
+    <t>- Chức danh công việc:</t>
+  </si>
+  <si>
+    <t>Công nhân may công nghiệp</t>
+  </si>
+  <si>
+    <t>- Công việc phải làm:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thực hiện theo bảng mô tả công việc và Các công việc liên quan khác dưới sự phân công  của người </t>
+  </si>
+  <si>
+    <t>quản lý trực tiếp.</t>
+  </si>
+  <si>
+    <t>ĐIỀU 2: THỜI GIAN LÀM VIỆC, THỜI GIAN NGHỈ NGƠI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Thời gian làm việc, làm thêm giờ và thời gian nghỉ ngơi theo nội quy, thỏa ước lao động tập thể của công ty và quy định của </t>
+  </si>
+  <si>
+    <t>pháp luật.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Nghỉ lễ, Tết, việc riêng có hưởng lương: theo quy định của pháp luật và nội quy của công ty. </t>
+  </si>
+  <si>
+    <t>ĐIỀU 3: TIỀN LƯƠNG VÀ CÁC CHẾ ĐỘ PHÚC LỢI</t>
+  </si>
+  <si>
+    <t>1. TIỀN LƯƠNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Mức lương: </t>
+  </si>
+  <si>
+    <t>5,573,000 VNĐ/ tháng</t>
+  </si>
+  <si>
+    <t>- Phụ cấp lương:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Các khoản bổ sung khác: </t>
+  </si>
+  <si>
+    <t>Theo Thỏa ước lao động tập thể, và các thông báo, quy định cụ thể của Công ty (nếu có)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiền lương được trả sau khi làm đủ số ngày công mỗi tháng dương lịch (người lao động không làm đủ ngày công trong một (01) </t>
+  </si>
+  <si>
+    <t>tháng thì tiền lương được hưởng sẽ là mức lương trừ đi tiền lương ngày nghỉ).</t>
+  </si>
+  <si>
+    <t>2. CÁC CHẾ ĐỘ PHÚC LỢI KHÁC</t>
+  </si>
+  <si>
+    <t>- Khen thưởng :</t>
+  </si>
+  <si>
+    <t>Người lao động được khuyến khích bằng vật chất và tinh thần khi có thành tích trong công tác hoặc theo quy định của công ty</t>
+  </si>
+  <si>
+    <t>Nếu người lao động không còn tiếp tục làm việc hoặc có đơn xin nghỉ việc đến ngày phát thưởng thì sẽ không được lĩnh thưởng_x000D_</t>
+  </si>
+  <si>
+    <t>- Tiền hỗ trợ xăng xe/ nhà ở, con nhỏ, thăm hỏi hiếu hỉ, ...:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thực hiện theo Thỏa ước lao động tập thể và các thông báo </t>
+  </si>
+  <si>
+    <t>cụ thể của Công ty.</t>
+  </si>
+  <si>
+    <t>3.  HÌNH THỨC TRẢ LƯƠNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Người lao động được trả lương theo lương thời gian và theo lương tháng. Hàng tháng tiền lương được chuyển khoản trực tiếp </t>
+  </si>
+  <si>
+    <t>vào tài khoản cá nhân của người lao động. Người lao động được nhận phiếu lương từng tháng từ phòng kế toán.</t>
+  </si>
+  <si>
+    <t>4. NGÀY TRẢ LƯƠNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Người lao động được trả lương theo tháng vào ngày 10 của tháng tiếp theo. Nếu ngày trả lương trùng vào ngày chủ nhật thì </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lương sẽ được trả vào ngày 11. Trường hợp đặc biệt nếu ngày trả lương rơi vào dịp nghỉ lễ, Tết thì công ty sẽ sắp xếp thời gian </t>
+  </si>
+  <si>
+    <t>thanh toán phù hợp và có thông báo trước cho người lao động.</t>
+  </si>
+  <si>
+    <t>5. CHẾ ĐỘ NÂNG BẬC, NÂNG LƯƠNG</t>
+  </si>
+  <si>
+    <t>Thực hiện theo quy chế của công ty, thỏa ước lao động tập thể và theo quy định của chính phủ (nếu có)</t>
+  </si>
+  <si>
+    <t>Mức lương nêu trên có thể được thay đổi theo chính sách nâng bậc tay nghề của công ty hoặc trong trường hợp Chính phủ điều</t>
+  </si>
+  <si>
+    <t>chỉnh mức lương tối thiểu vùng (nếu có). Trong trường hợp đó, công ty sẽ thông báo cho người lao động biết và mức lương, phụ</t>
+  </si>
+  <si>
+    <t>cấp (nếu có) sẽ tự động thay đổi theo quy định mới</t>
+  </si>
+  <si>
+    <t>6. TRANG BỊ BẢO HỘ LAO ĐỘNG</t>
+  </si>
+  <si>
+    <t>Người lao động được cấp phát trang thiết bị bảo hộ lao động theo chính sách cấp phát bảo hộ lao động của công ty.</t>
+  </si>
+  <si>
+    <t>7. BẢO HIỂM XÃ HỘI, BẢO HIỂM THẤT NGHIỆP, BẢO HIỂM Y TẾ, BẢO HIỂM TAI NẠN LAO ĐỘNG -																						_x000D_</t>
+  </si>
+  <si>
+    <t>BỆNH NGHỀ NGHIỆP</t>
+  </si>
+  <si>
+    <t>8. ĐÀO TẠO, BỒI DƯỠNG, NÂNG CAO TRÌNH ĐỘ KỸ NĂNG NGHỀ</t>
+  </si>
+  <si>
+    <t>Thực hiện theo quy định và chính sách đào tạo - phát triển của công ty.</t>
+  </si>
+  <si>
+    <t>4.1. Quyền lợi</t>
+  </si>
+  <si>
+    <t>- Được làm việc theo hợp đồng lao động và không bị phân biệt đối xử.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-  Hưởng lương phù hợp với trình độ kỹ năng nghề trên cơ sở thoả thuận với người sử dụng lao động; được bảo hộ lao động, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">làm việc trong điều kiện bảo đảm về an toàn lao động, vệ sinh lao động; nghỉ theo chế độ, nghỉ hằng năm có lương và được </t>
+  </si>
+  <si>
+    <t>hưởng phúc lợi tập thể.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Thành lập, gia nhập, hoạt động công đoàn, tổ chức nghề nghiệp và tổ chức khác theo quy định của pháp luật, ; yêu cầu và </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tham gia đối thoại với người sử dụng lao động, thực hiện quy chế dân chủ và được tham vấn tại nơi làm việc để bảo vệ quyền </t>
+  </si>
+  <si>
+    <t>và lợi ích hợp pháp của mình; tham gia quản lý theo nội quy của người sử dụng lao động.</t>
+  </si>
+  <si>
+    <t>-  Đơn phương chấm dứt hợp đồng lao động theo quy định của pháp luật.</t>
+  </si>
+  <si>
+    <t>- Các quyền khác theo quy định của pháp luật.</t>
+  </si>
+  <si>
+    <t>4.2. Nghĩa vụ</t>
+  </si>
+  <si>
+    <t>- Tuân thủ nội quy lao động, các quy định về tác phong làm việc, trật tự an ninh, qui định về hút thuốc, phòng chống cháy nổ,</t>
+  </si>
+  <si>
+    <t>an toàn vệ sinh lao động, kỷ luật lao động …</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Tuân thủ lệnh điều hành sản xuất – kinh doanh, các yêu cầu / quy định về sản xuất, chất lượng, an toàn sản phẩm, các quy </t>
+  </si>
+  <si>
+    <t>định của khách hàng, của tập đoàn, các quy định của bộ phận.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Hoàn thành công việc được giao, thực hiện theo sự phân công yêu cầu của bộ phận, người quản lý. </t>
+  </si>
+  <si>
+    <t>- Bồi thường thiệt hại: Theo Nội quy công ty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Về thuế: Người lao động chịu trách nhiệm nộp thuế thu nhập cá nhân của mình (nếu có). Trong bất kỳ hoàn cảnh nào, vì bất </t>
+  </si>
+  <si>
+    <t>cứ lý do gì, người lao động phải đảm bảo rằng Công ty sẽ không chịu thiệt hại nào phát sinh từ việc nộp thuế thu nhập cá nhân</t>
+  </si>
+  <si>
+    <t>của mình.</t>
+  </si>
+  <si>
+    <t>-  Về thời gian báo trước khi muốn chấm dứt hợp đồng lao động</t>
+  </si>
+  <si>
+    <t>Thời gian báo trước ít nhất là ba (03) ngày.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nếu bên nào vi phạm thời hạn báo trước thì bên vi phạm sẽ phải bồi thường cho bên kia một khoản tiền lương tương ứng với </t>
+  </si>
+  <si>
+    <t>tiền lương của người lao động trong thời gian không báo trước.</t>
+  </si>
+  <si>
+    <t>Quy định về thời gian báo trước nêu trên không áp dụng trong trường hợp người lao động bị xử lý kỷ luật sa thải trước và thực</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hiện theo nội quy của Công ty.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Ngoài những điều khoản nêu trong hợp đồng này, người lao động phải tuân thủ các quy định trong Nội quy của công ty, </t>
+  </si>
+  <si>
+    <t>Thỏa ước lao động tập thể và các quy chế khác.</t>
+  </si>
+  <si>
+    <t>ĐIỀU 5: NGHĨA VỤ VÀ QUYỀN HẠN CỦA NGƯỜI SỬ DỤNG LAO ĐỘNG</t>
+  </si>
+  <si>
+    <t>5.1. Quyền hạn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Người sử dụng lao động có các quyền sau: </t>
+  </si>
+  <si>
+    <t>- Tuyển dụng, bố trí, điều hành, điều chuyển lao động theo nhu cầu sản xuất, kinh doanh.</t>
+  </si>
+  <si>
+    <t>- Có quyền tạm hoãn, chấm dứt hợp đồng thử việc, kỷ luật người lao động theo quy định của pháp luật, thỏa ước lao động tập</t>
+  </si>
+  <si>
+    <t>thể và nội quy Công ty.</t>
+  </si>
+  <si>
+    <t>- Thực hiện các quy định của pháp luật về lao động, pháp luật về bảo hiểm xã hội và pháp luật về bảo hiểm y tế.</t>
+  </si>
+  <si>
+    <t>5.2. Nghĩa vụ</t>
+  </si>
+  <si>
+    <t>- Bảo đảm việc làm và thực hiện hợp đồng lao động, thỏa ước lao động tập thể và thỏa thuận khác với người lao động</t>
+  </si>
+  <si>
+    <t>tôn trọng danh dự, nhân phẩm của người lao động .</t>
+  </si>
+  <si>
+    <t>- Chịu trách nhiệm thanh toán đầy đủ, đúng hạn các chế độ và quyền lợi cho người lao động theo hợp đồng lao động, thỏa ước</t>
+  </si>
+  <si>
+    <t>lao động tập thể.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ĐIỀU 6: ĐIỀU KHOẢN THI HÀNH </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Những vấn đề về lao động không ghi trong hợp đồng này thì áp dụng theo quy định của Nội quy công ty, Thoả ước lao động </t>
+  </si>
+  <si>
+    <t>tập thể hoặc quy định của pháp luật có liên quan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hợp đồng lao động này được làm thành hai (02) bản có giá trị ngang nhau, mỗi bên giữ một (01) bản. Trong trường hợp có bất </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kỳ sửa đổi, bổ sung thì hai bên sẽ ký kết phụ lục hợp đồng. Khi hai bên ký kết Phụ lục hợp đồng lao động thì nội dung của Phụ </t>
+  </si>
+  <si>
+    <t>lục hợp đồng lao động cũng có giá trị như các nội dung của bản hợp đồng này.</t>
+  </si>
+  <si>
+    <t>Chữ ký người lao động</t>
+  </si>
+  <si>
+    <t>Thay mặt Công ty CP Sản xuất Nam Thuận</t>
+  </si>
+  <si>
+    <t>(Ký và ghi rõ họ tên)</t>
+  </si>
+  <si>
+    <t>…………………………………………..</t>
+  </si>
+  <si>
+    <t>Người được uỷ quyền</t>
+  </si>
+  <si>
+    <t>Họ tên:</t>
+  </si>
+  <si>
+    <t>Vị trí: Trưởng phòng Hành chính Nhân sự</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Người lao động ký hợp đồng lao động xác định thời hạn dưới 01 tháng không phải tham gia BHXH, BHYT, BHTN, BHTNLĐ - BNN. </t>
+  </si>
+  <si>
+    <t>ĐIỀU 4: NGHĨA VỤ VÀ QUYỀN HẠN CỦA NGƯỜI LAO ĐỘNG</t>
+  </si>
+  <si>
+    <t>Không</t>
+  </si>
+  <si>
+    <t>Thủy Sơn, Phường Thủy Đường, TP Thủy Nguyên, TP Hải Phòng</t>
+  </si>
+  <si>
+    <t>- Địa điểm làm việc: + Thủy Sơn, Phường Thủy Đường, TP Thủy Nguyên, TP Hải Phòng</t>
+  </si>
+  <si>
+    <t>Địa chỉ: Thuỷ Sơn - Thuỷ Đường - Thuỷ Nguyên - Hải Phòng
 ĐT: 02253.642.408</t>
-  </si>
-  <si>
-    <t>Độc lập - Tự do - Hạnh phúc</t>
-  </si>
-  <si>
-    <t>------------------------</t>
-  </si>
-  <si>
-    <t>Số: LC28D/13282</t>
-  </si>
-  <si>
-    <t>Hải Phòng, ngày 05 tháng 06 năm 2024</t>
-  </si>
-  <si>
-    <t>HỢP ĐỒNG LAO ĐỘNG</t>
-  </si>
-  <si>
-    <t>(Căn cứ vào BLLĐ 45/2019/QH 14 và NĐ 145/2020/NĐ-CP, TT 10/2020/TT-BLĐTBXH )</t>
-  </si>
-  <si>
-    <t>Chúng tôi, một bên là</t>
-  </si>
-  <si>
-    <t>Ông/Bà:</t>
-  </si>
-  <si>
-    <t>VŨ THỊ HIỀN</t>
-  </si>
-  <si>
-    <t>Quốc tịch:</t>
-  </si>
-  <si>
-    <t>VIỆT NAM</t>
-  </si>
-  <si>
-    <t>Chức vụ:</t>
-  </si>
-  <si>
-    <t>Trưởng phòng Hành chính Nhân sự</t>
-  </si>
-  <si>
-    <t>Sinh ngày:</t>
-  </si>
-  <si>
-    <t>05/09/1990           Giới tính: Nữ</t>
-  </si>
-  <si>
-    <t>Địa chỉ thường trú:</t>
-  </si>
-  <si>
-    <t>Quyết Tiến 3, An Thắng, An Lão, Hải Phòng</t>
-  </si>
-  <si>
-    <t>Số CCCD:</t>
-  </si>
-  <si>
-    <t>031190008508</t>
-  </si>
-  <si>
-    <t>Cấp ngày:</t>
-  </si>
-  <si>
-    <t>02/03/2022</t>
-  </si>
-  <si>
-    <t>Nơi cấp:</t>
-  </si>
-  <si>
-    <t>Cục cảnh sát</t>
-  </si>
-  <si>
-    <t>Đại diện cho:</t>
-  </si>
-  <si>
-    <t>Địa chỉ:</t>
-  </si>
-  <si>
-    <t>Thôn Rực Liễn, xã Thủy Sơn, huyện Thủy Nguyên, TP Hải Phòng</t>
-  </si>
-  <si>
-    <t>Điện thoại:</t>
-  </si>
-  <si>
-    <t>02253642408</t>
-  </si>
-  <si>
-    <t>Fax:</t>
-  </si>
-  <si>
-    <t>02253642407</t>
-  </si>
-  <si>
-    <t>Và một bên là:</t>
-  </si>
-  <si>
-    <t>BÙI THỊ HUYỀN</t>
-  </si>
-  <si>
-    <t>VIỆT NAM</t>
-  </si>
-  <si>
-    <t>10/03/1991</t>
-  </si>
-  <si>
-    <t>Giới tính:</t>
-  </si>
-  <si>
-    <t>Nữ</t>
-  </si>
-  <si>
-    <t>Thôn 1, Cao Nhân, Thủy Nguyên, Hải Phòng</t>
-  </si>
-  <si>
-    <t>Số CCCD: 31191003277</t>
-  </si>
-  <si>
-    <t>09/08/2021</t>
-  </si>
-  <si>
-    <t>Thỏa thuận ký kết hợp đồng lao động và cam kết làm đúng những điều khoản sau đây:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ĐIỀU 1: HỢP ĐỒNG VÀ CÔNG VIỆC HỢP ĐỒNG </t>
-  </si>
-  <si>
-    <t>- Thời hạn hợp đồng:</t>
-  </si>
-  <si>
-    <t>Hợp đồng xác định thời hạn 28 ngày</t>
-  </si>
-  <si>
-    <t>Từ ngày 05 tháng 06 năm 2024 đến hết ngày 02 tháng 07 năm 2024</t>
-  </si>
-  <si>
-    <t>- Địa điểm làm việc: + Thôn Rực Liễn, xã Thủy Sơn, huyện Thủy Nguyên, TP Hải Phòng</t>
-  </si>
-  <si>
-    <t>+ Các địa điểm khác theo sự phân công của Công ty theo yêu cầu công việc</t>
-  </si>
-  <si>
-    <t>- Chức danh công việc:</t>
-  </si>
-  <si>
-    <t>Công nhân may công nghiệp</t>
-  </si>
-  <si>
-    <t>- Công việc phải làm:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thực hiện theo bảng mô tả công việc và Các công việc liên quan khác dưới sự phân công  của người </t>
-  </si>
-  <si>
-    <t>quản lý trực tiếp.</t>
-  </si>
-  <si>
-    <t>ĐIỀU 2: THỜI GIAN LÀM VIỆC, THỜI GIAN NGHỈ NGƠI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Thời gian làm việc, làm thêm giờ và thời gian nghỉ ngơi theo nội quy, thỏa ước lao động tập thể của công ty và quy định của </t>
-  </si>
-  <si>
-    <t>pháp luật.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Nghỉ lễ, Tết, việc riêng có hưởng lương: theo quy định của pháp luật và nội quy của công ty. </t>
-  </si>
-  <si>
-    <t>ĐIỀU 3: TIỀN LƯƠNG VÀ CÁC CHẾ ĐỘ PHÚC LỢI</t>
-  </si>
-  <si>
-    <t>1. TIỀN LƯƠNG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Mức lương: </t>
-  </si>
-  <si>
-    <t>5,573,000 VNĐ/ tháng</t>
-  </si>
-  <si>
-    <t>- Phụ cấp lương:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Các khoản bổ sung khác: </t>
-  </si>
-  <si>
-    <t>Theo Thỏa ước lao động tập thể, và các thông báo, quy định cụ thể của Công ty (nếu có)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiền lương được trả sau khi làm đủ số ngày công mỗi tháng dương lịch (người lao động không làm đủ ngày công trong một (01) </t>
-  </si>
-  <si>
-    <t>tháng thì tiền lương được hưởng sẽ là mức lương trừ đi tiền lương ngày nghỉ).</t>
-  </si>
-  <si>
-    <t>2. CÁC CHẾ ĐỘ PHÚC LỢI KHÁC</t>
-  </si>
-  <si>
-    <t>- Khen thưởng :</t>
-  </si>
-  <si>
-    <t>Người lao động được khuyến khích bằng vật chất và tinh thần khi có thành tích trong công tác hoặc theo quy định của công ty</t>
-  </si>
-  <si>
-    <t>Nếu người lao động không còn tiếp tục làm việc hoặc có đơn xin nghỉ việc đến ngày phát thưởng thì sẽ không được lĩnh thưởng_x000D_</t>
-  </si>
-  <si>
-    <t>- Tiền hỗ trợ xăng xe/ nhà ở, con nhỏ, thăm hỏi hiếu hỉ, ...:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">thực hiện theo Thỏa ước lao động tập thể và các thông báo </t>
-  </si>
-  <si>
-    <t>cụ thể của Công ty.</t>
-  </si>
-  <si>
-    <t>3.  HÌNH THỨC TRẢ LƯƠNG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Người lao động được trả lương theo lương thời gian và theo lương tháng. Hàng tháng tiền lương được chuyển khoản trực tiếp </t>
-  </si>
-  <si>
-    <t>vào tài khoản cá nhân của người lao động. Người lao động được nhận phiếu lương từng tháng từ phòng kế toán.</t>
-  </si>
-  <si>
-    <t>4. NGÀY TRẢ LƯƠNG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Người lao động được trả lương theo tháng vào ngày 10 của tháng tiếp theo. Nếu ngày trả lương trùng vào ngày chủ nhật thì </t>
-  </si>
-  <si>
-    <t xml:space="preserve">lương sẽ được trả vào ngày 11. Trường hợp đặc biệt nếu ngày trả lương rơi vào dịp nghỉ lễ, Tết thì công ty sẽ sắp xếp thời gian </t>
-  </si>
-  <si>
-    <t>thanh toán phù hợp và có thông báo trước cho người lao động.</t>
-  </si>
-  <si>
-    <t>5. CHẾ ĐỘ NÂNG BẬC, NÂNG LƯƠNG</t>
-  </si>
-  <si>
-    <t>Thực hiện theo quy chế của công ty, thỏa ước lao động tập thể và theo quy định của chính phủ (nếu có)</t>
-  </si>
-  <si>
-    <t>Mức lương nêu trên có thể được thay đổi theo chính sách nâng bậc tay nghề của công ty hoặc trong trường hợp Chính phủ điều</t>
-  </si>
-  <si>
-    <t>chỉnh mức lương tối thiểu vùng (nếu có). Trong trường hợp đó, công ty sẽ thông báo cho người lao động biết và mức lương, phụ</t>
-  </si>
-  <si>
-    <t>cấp (nếu có) sẽ tự động thay đổi theo quy định mới</t>
-  </si>
-  <si>
-    <t>6. TRANG BỊ BẢO HỘ LAO ĐỘNG</t>
-  </si>
-  <si>
-    <t>Người lao động được cấp phát trang thiết bị bảo hộ lao động theo chính sách cấp phát bảo hộ lao động của công ty.</t>
-  </si>
-  <si>
-    <t>7. BẢO HIỂM XÃ HỘI, BẢO HIỂM THẤT NGHIỆP, BẢO HIỂM Y TẾ, BẢO HIỂM TAI NẠN LAO ĐỘNG -																						_x000D_</t>
-  </si>
-  <si>
-    <t>BỆNH NGHỀ NGHIỆP</t>
-  </si>
-  <si>
-    <t>8. ĐÀO TẠO, BỒI DƯỠNG, NÂNG CAO TRÌNH ĐỘ KỸ NĂNG NGHỀ</t>
-  </si>
-  <si>
-    <t>Thực hiện theo quy định và chính sách đào tạo - phát triển của công ty.</t>
-  </si>
-  <si>
-    <t>4.1. Quyền lợi</t>
-  </si>
-  <si>
-    <t>- Được làm việc theo hợp đồng lao động và không bị phân biệt đối xử.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-  Hưởng lương phù hợp với trình độ kỹ năng nghề trên cơ sở thoả thuận với người sử dụng lao động; được bảo hộ lao động, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">làm việc trong điều kiện bảo đảm về an toàn lao động, vệ sinh lao động; nghỉ theo chế độ, nghỉ hằng năm có lương và được </t>
-  </si>
-  <si>
-    <t>hưởng phúc lợi tập thể.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Thành lập, gia nhập, hoạt động công đoàn, tổ chức nghề nghiệp và tổ chức khác theo quy định của pháp luật, ; yêu cầu và </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tham gia đối thoại với người sử dụng lao động, thực hiện quy chế dân chủ và được tham vấn tại nơi làm việc để bảo vệ quyền </t>
-  </si>
-  <si>
-    <t>và lợi ích hợp pháp của mình; tham gia quản lý theo nội quy của người sử dụng lao động.</t>
-  </si>
-  <si>
-    <t>-  Đơn phương chấm dứt hợp đồng lao động theo quy định của pháp luật.</t>
-  </si>
-  <si>
-    <t>- Các quyền khác theo quy định của pháp luật.</t>
-  </si>
-  <si>
-    <t>4.2. Nghĩa vụ</t>
-  </si>
-  <si>
-    <t>- Tuân thủ nội quy lao động, các quy định về tác phong làm việc, trật tự an ninh, qui định về hút thuốc, phòng chống cháy nổ,</t>
-  </si>
-  <si>
-    <t>an toàn vệ sinh lao động, kỷ luật lao động …</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Tuân thủ lệnh điều hành sản xuất – kinh doanh, các yêu cầu / quy định về sản xuất, chất lượng, an toàn sản phẩm, các quy </t>
-  </si>
-  <si>
-    <t>định của khách hàng, của tập đoàn, các quy định của bộ phận.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Hoàn thành công việc được giao, thực hiện theo sự phân công yêu cầu của bộ phận, người quản lý. </t>
-  </si>
-  <si>
-    <t>- Bồi thường thiệt hại: Theo Nội quy công ty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Về thuế: Người lao động chịu trách nhiệm nộp thuế thu nhập cá nhân của mình (nếu có). Trong bất kỳ hoàn cảnh nào, vì bất </t>
-  </si>
-  <si>
-    <t>cứ lý do gì, người lao động phải đảm bảo rằng Công ty sẽ không chịu thiệt hại nào phát sinh từ việc nộp thuế thu nhập cá nhân</t>
-  </si>
-  <si>
-    <t>của mình.</t>
-  </si>
-  <si>
-    <t>-  Về thời gian báo trước khi muốn chấm dứt hợp đồng lao động</t>
-  </si>
-  <si>
-    <t>Thời gian báo trước ít nhất là ba (03) ngày.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nếu bên nào vi phạm thời hạn báo trước thì bên vi phạm sẽ phải bồi thường cho bên kia một khoản tiền lương tương ứng với </t>
-  </si>
-  <si>
-    <t>tiền lương của người lao động trong thời gian không báo trước.</t>
-  </si>
-  <si>
-    <t>Quy định về thời gian báo trước nêu trên không áp dụng trong trường hợp người lao động bị xử lý kỷ luật sa thải trước và thực</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> hiện theo nội quy của Công ty.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Ngoài những điều khoản nêu trong hợp đồng này, người lao động phải tuân thủ các quy định trong Nội quy của công ty, </t>
-  </si>
-  <si>
-    <t>Thỏa ước lao động tập thể và các quy chế khác.</t>
-  </si>
-  <si>
-    <t>ĐIỀU 5: NGHĨA VỤ VÀ QUYỀN HẠN CỦA NGƯỜI SỬ DỤNG LAO ĐỘNG</t>
-  </si>
-  <si>
-    <t>5.1. Quyền hạn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Người sử dụng lao động có các quyền sau: </t>
-  </si>
-  <si>
-    <t>- Tuyển dụng, bố trí, điều hành, điều chuyển lao động theo nhu cầu sản xuất, kinh doanh.</t>
-  </si>
-  <si>
-    <t>- Có quyền tạm hoãn, chấm dứt hợp đồng thử việc, kỷ luật người lao động theo quy định của pháp luật, thỏa ước lao động tập</t>
-  </si>
-  <si>
-    <t>thể và nội quy Công ty.</t>
-  </si>
-  <si>
-    <t>- Thực hiện các quy định của pháp luật về lao động, pháp luật về bảo hiểm xã hội và pháp luật về bảo hiểm y tế.</t>
-  </si>
-  <si>
-    <t>5.2. Nghĩa vụ</t>
-  </si>
-  <si>
-    <t>- Bảo đảm việc làm và thực hiện hợp đồng lao động, thỏa ước lao động tập thể và thỏa thuận khác với người lao động</t>
-  </si>
-  <si>
-    <t>tôn trọng danh dự, nhân phẩm của người lao động .</t>
-  </si>
-  <si>
-    <t>- Chịu trách nhiệm thanh toán đầy đủ, đúng hạn các chế độ và quyền lợi cho người lao động theo hợp đồng lao động, thỏa ước</t>
-  </si>
-  <si>
-    <t>lao động tập thể.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ĐIỀU 6: ĐIỀU KHOẢN THI HÀNH </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Những vấn đề về lao động không ghi trong hợp đồng này thì áp dụng theo quy định của Nội quy công ty, Thoả ước lao động </t>
-  </si>
-  <si>
-    <t>tập thể hoặc quy định của pháp luật có liên quan.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hợp đồng lao động này được làm thành hai (02) bản có giá trị ngang nhau, mỗi bên giữ một (01) bản. Trong trường hợp có bất </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kỳ sửa đổi, bổ sung thì hai bên sẽ ký kết phụ lục hợp đồng. Khi hai bên ký kết Phụ lục hợp đồng lao động thì nội dung của Phụ </t>
-  </si>
-  <si>
-    <t>lục hợp đồng lao động cũng có giá trị như các nội dung của bản hợp đồng này.</t>
-  </si>
-  <si>
-    <t>Chữ ký người lao động</t>
-  </si>
-  <si>
-    <t>Thay mặt Công ty CP Sản xuất Nam Thuận</t>
-  </si>
-  <si>
-    <t>(Ký và ghi rõ họ tên)</t>
-  </si>
-  <si>
-    <t>…………………………………………..</t>
-  </si>
-  <si>
-    <t>Người được uỷ quyền</t>
-  </si>
-  <si>
-    <t>Họ tên:</t>
-  </si>
-  <si>
-    <t>Vị trí: Trưởng phòng Hành chính Nhân sự</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Người lao động ký hợp đồng lao động xác định thời hạn dưới 01 tháng không phải tham gia BHXH, BHYT, BHTN, BHTNLĐ - BNN. </t>
-  </si>
-  <si>
-    <t>ĐIỀU 4: NGHĨA VỤ VÀ QUYỀN HẠN CỦA NGƯỜI LAO ĐỘNG</t>
-  </si>
-  <si>
-    <t>Không</t>
   </si>
 </sst>
 </file>
@@ -574,7 +574,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -620,6 +620,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -635,9 +638,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -646,6 +646,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1120,8 +1123,8 @@
   </sheetPr>
   <dimension ref="A1:X127"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67:X67"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1169,7 +1172,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="6" t="s">
-        <v>2</v>
+        <v>147</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -1179,7 +1182,7 @@
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
       <c r="M2" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
@@ -1199,7 +1202,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
@@ -1209,7 +1212,7 @@
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
@@ -1229,7 +1232,7 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -1239,7 +1242,7 @@
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
       <c r="M4" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
@@ -1281,7 +1284,7 @@
     </row>
     <row r="6" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -1309,7 +1312,7 @@
     </row>
     <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -1364,7 +1367,7 @@
     <row r="9" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
@@ -1392,11 +1395,11 @@
     <row r="10" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
@@ -1408,12 +1411,12 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
       <c r="N10" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O10" s="13"/>
       <c r="P10" s="13"/>
       <c r="Q10" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="R10" s="12"/>
       <c r="S10" s="12"/>
@@ -1426,11 +1429,11 @@
     <row r="11" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
@@ -1442,12 +1445,12 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
       <c r="N11" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
       <c r="Q11" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R11" s="13"/>
       <c r="S11" s="13"/>
@@ -1460,13 +1463,13 @@
     <row r="12" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
@@ -1490,33 +1493,33 @@
     <row r="13" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
       <c r="E13" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
       <c r="I13" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M13" s="13"/>
       <c r="N13" s="13"/>
       <c r="O13" s="13"/>
       <c r="P13" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q13" s="13"/>
       <c r="R13" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S13" s="13"/>
       <c r="T13" s="13"/>
@@ -1528,7 +1531,7 @@
     <row r="14" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -1558,11 +1561,11 @@
     <row r="15" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13" t="s">
-        <v>28</v>
+        <v>145</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
@@ -1588,12 +1591,12 @@
     <row r="16" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
       <c r="E16" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
@@ -1604,11 +1607,11 @@
       <c r="L16" s="14"/>
       <c r="M16" s="14"/>
       <c r="N16" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O16" s="13"/>
       <c r="P16" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Q16" s="14"/>
       <c r="R16" s="14"/>
@@ -1622,7 +1625,7 @@
     <row r="17" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
@@ -1650,11 +1653,11 @@
     <row r="18" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
@@ -1666,12 +1669,12 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
       <c r="N18" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O18" s="13"/>
       <c r="P18" s="13"/>
       <c r="Q18" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="R18" s="12"/>
       <c r="S18" s="12"/>
@@ -1684,12 +1687,12 @@
     <row r="19" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
       <c r="E19" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
@@ -1700,12 +1703,12 @@
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
       <c r="N19" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O19" s="13"/>
       <c r="P19" s="13"/>
       <c r="Q19" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="R19" s="13"/>
       <c r="S19" s="13"/>
@@ -1718,13 +1721,13 @@
     <row r="20" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
       <c r="F20" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
@@ -1748,7 +1751,7 @@
     <row r="21" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
@@ -1757,22 +1760,22 @@
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
       <c r="I21" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
       <c r="L21" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M21" s="13"/>
       <c r="N21" s="13"/>
       <c r="O21" s="13"/>
       <c r="P21" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q21" s="13"/>
       <c r="R21" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S21" s="13"/>
       <c r="T21" s="13"/>
@@ -1784,7 +1787,7 @@
     <row r="22" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
@@ -1812,7 +1815,7 @@
     <row r="23" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
@@ -1840,7 +1843,7 @@
     <row r="24" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
@@ -1868,7 +1871,7 @@
     <row r="25" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
@@ -1876,7 +1879,7 @@
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
       <c r="H25" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
@@ -1898,7 +1901,7 @@
     <row r="26" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
@@ -1925,8 +1928,8 @@
     </row>
     <row r="27" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
-      <c r="B27" s="13" t="s">
-        <v>47</v>
+      <c r="B27" s="15" t="s">
+        <v>146</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
@@ -1958,7 +1961,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
@@ -1982,14 +1985,14 @@
     <row r="29" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
@@ -2012,14 +2015,14 @@
     <row r="30" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
@@ -2042,7 +2045,7 @@
     <row r="31" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
@@ -2070,7 +2073,7 @@
     <row r="32" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
@@ -2098,7 +2101,7 @@
     <row r="33" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
@@ -2126,7 +2129,7 @@
     <row r="34" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
@@ -2154,7 +2157,7 @@
     <row r="35" spans="1:24" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C35" s="13"/>
       <c r="D35" s="13"/>
@@ -2208,7 +2211,7 @@
     <row r="37" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
@@ -2235,73 +2238,73 @@
     </row>
     <row r="38" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
-      <c r="B38" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="15"/>
-      <c r="P38" s="15"/>
-      <c r="Q38" s="15"/>
-      <c r="R38" s="15"/>
-      <c r="S38" s="15"/>
-      <c r="T38" s="15"/>
-      <c r="U38" s="15"/>
-      <c r="V38" s="15"/>
-      <c r="W38" s="15"/>
-      <c r="X38" s="15"/>
+      <c r="B38" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="16"/>
+      <c r="S38" s="16"/>
+      <c r="T38" s="16"/>
+      <c r="U38" s="16"/>
+      <c r="V38" s="16"/>
+      <c r="W38" s="16"/>
+      <c r="X38" s="16"/>
     </row>
     <row r="39" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
-      <c r="G39" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="H39" s="16"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="16"/>
-      <c r="K39" s="16"/>
-      <c r="L39" s="16"/>
-      <c r="M39" s="16"/>
-      <c r="N39" s="16"/>
-      <c r="O39" s="16"/>
-      <c r="P39" s="16"/>
-      <c r="Q39" s="16"/>
-      <c r="R39" s="16"/>
-      <c r="S39" s="16"/>
-      <c r="T39" s="16"/>
-      <c r="U39" s="16"/>
-      <c r="V39" s="16"/>
-      <c r="W39" s="16"/>
-      <c r="X39" s="16"/>
+      <c r="G39" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="17"/>
+      <c r="P39" s="17"/>
+      <c r="Q39" s="17"/>
+      <c r="R39" s="17"/>
+      <c r="S39" s="17"/>
+      <c r="T39" s="17"/>
+      <c r="U39" s="17"/>
+      <c r="V39" s="17"/>
+      <c r="W39" s="17"/>
+      <c r="X39" s="17"/>
     </row>
     <row r="40" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
-      <c r="B40" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
+      <c r="B40" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
       <c r="F40" s="2"/>
       <c r="G40" s="14" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H40" s="14"/>
       <c r="I40" s="14"/>
@@ -2309,17 +2312,17 @@
       <c r="K40" s="14"/>
       <c r="L40" s="14"/>
       <c r="M40" s="14"/>
-      <c r="N40" s="18"/>
-      <c r="O40" s="18"/>
-      <c r="P40" s="18"/>
-      <c r="Q40" s="18"/>
-      <c r="R40" s="18"/>
-      <c r="S40" s="18"/>
-      <c r="T40" s="18"/>
-      <c r="U40" s="18"/>
-      <c r="V40" s="18"/>
-      <c r="W40" s="18"/>
-      <c r="X40" s="18"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="19"/>
+      <c r="R40" s="19"/>
+      <c r="S40" s="19"/>
+      <c r="T40" s="19"/>
+      <c r="U40" s="19"/>
+      <c r="V40" s="19"/>
+      <c r="W40" s="19"/>
+      <c r="X40" s="19"/>
     </row>
     <row r="41" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
@@ -2350,7 +2353,7 @@
     <row r="42" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
@@ -2358,7 +2361,7 @@
       <c r="F42" s="12"/>
       <c r="G42" s="12"/>
       <c r="H42" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I42" s="13"/>
       <c r="J42" s="13"/>
@@ -2380,7 +2383,7 @@
     <row r="43" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C43" s="13"/>
       <c r="D43" s="13"/>
@@ -2408,7 +2411,7 @@
     <row r="44" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C44" s="13"/>
       <c r="D44" s="13"/>
@@ -2436,7 +2439,7 @@
     <row r="45" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C45" s="12"/>
       <c r="D45" s="12"/>
@@ -2464,7 +2467,7 @@
     <row r="46" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
@@ -2492,7 +2495,7 @@
     <row r="47" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C47" s="13"/>
       <c r="D47" s="13"/>
@@ -2519,8 +2522,8 @@
     </row>
     <row r="48" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
-      <c r="B48" s="19" t="s">
-        <v>70</v>
+      <c r="B48" s="20" t="s">
+        <v>67</v>
       </c>
       <c r="C48" s="13"/>
       <c r="D48" s="13"/>
@@ -2548,7 +2551,7 @@
     <row r="49" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
@@ -2561,7 +2564,7 @@
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
       <c r="M49" s="13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N49" s="13"/>
       <c r="O49" s="13"/>
@@ -2578,7 +2581,7 @@
     <row r="50" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C50" s="13"/>
       <c r="D50" s="13"/>
@@ -2606,7 +2609,7 @@
     <row r="51" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C51" s="12"/>
       <c r="D51" s="12"/>
@@ -2634,7 +2637,7 @@
     <row r="52" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C52" s="13"/>
       <c r="D52" s="13"/>
@@ -2662,7 +2665,7 @@
     <row r="53" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C53" s="13"/>
       <c r="D53" s="13"/>
@@ -2690,7 +2693,7 @@
     <row r="54" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C54" s="12"/>
       <c r="D54" s="12"/>
@@ -2718,7 +2721,7 @@
     <row r="55" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C55" s="13"/>
       <c r="D55" s="13"/>
@@ -2746,7 +2749,7 @@
     <row r="56" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C56" s="13"/>
       <c r="D56" s="13"/>
@@ -2774,7 +2777,7 @@
     <row r="57" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C57" s="13"/>
       <c r="D57" s="13"/>
@@ -2802,7 +2805,7 @@
     <row r="58" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
       <c r="B58" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C58" s="12"/>
       <c r="D58" s="12"/>
@@ -2830,7 +2833,7 @@
     <row r="59" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C59" s="13"/>
       <c r="D59" s="13"/>
@@ -2858,7 +2861,7 @@
     <row r="60" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C60" s="13"/>
       <c r="D60" s="13"/>
@@ -2886,7 +2889,7 @@
     <row r="61" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C61" s="13"/>
       <c r="D61" s="13"/>
@@ -2914,7 +2917,7 @@
     <row r="62" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C62" s="13"/>
       <c r="D62" s="13"/>
@@ -2942,7 +2945,7 @@
     <row r="63" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C63" s="12"/>
       <c r="D63" s="12"/>
@@ -2970,7 +2973,7 @@
     <row r="64" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
       <c r="B64" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C64" s="13"/>
       <c r="D64" s="13"/>
@@ -2998,7 +3001,7 @@
     <row r="65" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="21" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C65" s="22"/>
       <c r="D65" s="22"/>
@@ -3026,7 +3029,7 @@
     <row r="66" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
       <c r="B66" s="22" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C66" s="22"/>
       <c r="D66" s="22"/>
@@ -3054,7 +3057,7 @@
     <row r="67" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
       <c r="B67" s="23" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C67" s="23"/>
       <c r="D67" s="23"/>
@@ -3082,7 +3085,7 @@
     <row r="68" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C68" s="12"/>
       <c r="D68" s="12"/>
@@ -3110,7 +3113,7 @@
     <row r="69" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C69" s="13"/>
       <c r="D69" s="13"/>
@@ -3138,7 +3141,7 @@
     <row r="70" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
       <c r="B70" s="12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C70" s="12"/>
       <c r="D70" s="12"/>
@@ -3166,7 +3169,7 @@
     <row r="71" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" s="12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C71" s="12"/>
       <c r="D71" s="12"/>
@@ -3194,7 +3197,7 @@
     <row r="72" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2"/>
       <c r="B72" s="13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C72" s="13"/>
       <c r="D72" s="13"/>
@@ -3222,7 +3225,7 @@
     <row r="73" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C73" s="13"/>
       <c r="D73" s="13"/>
@@ -3250,7 +3253,7 @@
     <row r="74" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2"/>
       <c r="B74" s="13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C74" s="13"/>
       <c r="D74" s="13"/>
@@ -3278,7 +3281,7 @@
     <row r="75" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
       <c r="B75" s="13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C75" s="13"/>
       <c r="D75" s="13"/>
@@ -3306,7 +3309,7 @@
     <row r="76" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
       <c r="B76" s="13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C76" s="13"/>
       <c r="D76" s="13"/>
@@ -3334,7 +3337,7 @@
     <row r="77" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2"/>
       <c r="B77" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C77" s="13"/>
       <c r="D77" s="13"/>
@@ -3362,7 +3365,7 @@
     <row r="78" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2"/>
       <c r="B78" s="13" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C78" s="13"/>
       <c r="D78" s="13"/>
@@ -3390,7 +3393,7 @@
     <row r="79" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
       <c r="B79" s="13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C79" s="13"/>
       <c r="D79" s="13"/>
@@ -3418,7 +3421,7 @@
     <row r="80" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2"/>
       <c r="B80" s="13" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C80" s="13"/>
       <c r="D80" s="13"/>
@@ -3445,36 +3448,36 @@
     </row>
     <row r="81" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2"/>
-      <c r="B81" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="C81" s="15"/>
-      <c r="D81" s="15"/>
-      <c r="E81" s="15"/>
-      <c r="F81" s="15"/>
-      <c r="G81" s="15"/>
-      <c r="H81" s="15"/>
-      <c r="I81" s="15"/>
-      <c r="J81" s="15"/>
-      <c r="K81" s="15"/>
-      <c r="L81" s="15"/>
-      <c r="M81" s="15"/>
-      <c r="N81" s="15"/>
-      <c r="O81" s="15"/>
-      <c r="P81" s="15"/>
-      <c r="Q81" s="15"/>
-      <c r="R81" s="15"/>
-      <c r="S81" s="15"/>
-      <c r="T81" s="15"/>
-      <c r="U81" s="15"/>
-      <c r="V81" s="15"/>
-      <c r="W81" s="15"/>
-      <c r="X81" s="15"/>
+      <c r="B81" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C81" s="16"/>
+      <c r="D81" s="16"/>
+      <c r="E81" s="16"/>
+      <c r="F81" s="16"/>
+      <c r="G81" s="16"/>
+      <c r="H81" s="16"/>
+      <c r="I81" s="16"/>
+      <c r="J81" s="16"/>
+      <c r="K81" s="16"/>
+      <c r="L81" s="16"/>
+      <c r="M81" s="16"/>
+      <c r="N81" s="16"/>
+      <c r="O81" s="16"/>
+      <c r="P81" s="16"/>
+      <c r="Q81" s="16"/>
+      <c r="R81" s="16"/>
+      <c r="S81" s="16"/>
+      <c r="T81" s="16"/>
+      <c r="U81" s="16"/>
+      <c r="V81" s="16"/>
+      <c r="W81" s="16"/>
+      <c r="X81" s="16"/>
     </row>
     <row r="82" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2"/>
       <c r="B82" s="13" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C82" s="13"/>
       <c r="D82" s="13"/>
@@ -3502,7 +3505,7 @@
     <row r="83" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2"/>
       <c r="B83" s="13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C83" s="13"/>
       <c r="D83" s="13"/>
@@ -3530,7 +3533,7 @@
     <row r="84" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2"/>
       <c r="B84" s="13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C84" s="13"/>
       <c r="D84" s="13"/>
@@ -3558,7 +3561,7 @@
     <row r="85" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2"/>
       <c r="B85" s="13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C85" s="13"/>
       <c r="D85" s="13"/>
@@ -3586,7 +3589,7 @@
     <row r="86" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2"/>
       <c r="B86" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C86" s="13"/>
       <c r="D86" s="13"/>
@@ -3614,7 +3617,7 @@
     <row r="87" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
       <c r="B87" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C87" s="13"/>
       <c r="D87" s="13"/>
@@ -3642,7 +3645,7 @@
     <row r="88" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2"/>
       <c r="B88" s="13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C88" s="13"/>
       <c r="D88" s="13"/>
@@ -3670,7 +3673,7 @@
     <row r="89" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2"/>
       <c r="B89" s="13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C89" s="13"/>
       <c r="D89" s="13"/>
@@ -3698,7 +3701,7 @@
     <row r="90" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2"/>
       <c r="B90" s="13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C90" s="13"/>
       <c r="D90" s="13"/>
@@ -3726,7 +3729,7 @@
     <row r="91" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2"/>
       <c r="B91" s="13" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C91" s="13"/>
       <c r="D91" s="13"/>
@@ -3754,7 +3757,7 @@
     <row r="92" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2"/>
       <c r="B92" s="13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C92" s="13"/>
       <c r="D92" s="13"/>
@@ -3782,7 +3785,7 @@
     <row r="93" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2"/>
       <c r="B93" s="13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C93" s="13"/>
       <c r="D93" s="13"/>
@@ -3810,7 +3813,7 @@
     <row r="94" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2"/>
       <c r="B94" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C94" s="13"/>
       <c r="D94" s="13"/>
@@ -3838,7 +3841,7 @@
     <row r="95" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2"/>
       <c r="B95" s="13" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C95" s="13"/>
       <c r="D95" s="13"/>
@@ -3866,7 +3869,7 @@
     <row r="96" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2"/>
       <c r="B96" s="13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C96" s="13"/>
       <c r="D96" s="13"/>
@@ -3894,7 +3897,7 @@
     <row r="97" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2"/>
       <c r="B97" s="13" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C97" s="13"/>
       <c r="D97" s="13"/>
@@ -3922,7 +3925,7 @@
     <row r="98" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2"/>
       <c r="B98" s="13" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C98" s="13"/>
       <c r="D98" s="13"/>
@@ -3976,7 +3979,7 @@
     <row r="100" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2"/>
       <c r="B100" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C100" s="12"/>
       <c r="D100" s="12"/>
@@ -4004,7 +4007,7 @@
     <row r="101" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2"/>
       <c r="B101" s="12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C101" s="12"/>
       <c r="D101" s="12"/>
@@ -4032,7 +4035,7 @@
     <row r="102" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2"/>
       <c r="B102" s="13" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C102" s="13"/>
       <c r="D102" s="13"/>
@@ -4060,7 +4063,7 @@
     <row r="103" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2"/>
       <c r="B103" s="13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C103" s="13"/>
       <c r="D103" s="13"/>
@@ -4088,7 +4091,7 @@
     <row r="104" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2"/>
       <c r="B104" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C104" s="13"/>
       <c r="D104" s="13"/>
@@ -4116,7 +4119,7 @@
     <row r="105" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2"/>
       <c r="B105" s="13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C105" s="13"/>
       <c r="D105" s="13"/>
@@ -4144,7 +4147,7 @@
     <row r="106" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2"/>
       <c r="B106" s="13" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C106" s="13"/>
       <c r="D106" s="13"/>
@@ -4172,7 +4175,7 @@
     <row r="107" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2"/>
       <c r="B107" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C107" s="12"/>
       <c r="D107" s="12"/>
@@ -4200,7 +4203,7 @@
     <row r="108" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2"/>
       <c r="B108" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C108" s="13"/>
       <c r="D108" s="13"/>
@@ -4228,7 +4231,7 @@
     <row r="109" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2"/>
       <c r="B109" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C109" s="13"/>
       <c r="D109" s="13"/>
@@ -4256,7 +4259,7 @@
     <row r="110" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2"/>
       <c r="B110" s="13" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C110" s="13"/>
       <c r="D110" s="13"/>
@@ -4284,7 +4287,7 @@
     <row r="111" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2"/>
       <c r="B111" s="13" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C111" s="13"/>
       <c r="D111" s="13"/>
@@ -4312,7 +4315,7 @@
     <row r="112" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2"/>
       <c r="B112" s="12" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C112" s="12"/>
       <c r="D112" s="12"/>
@@ -4340,7 +4343,7 @@
     <row r="113" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2"/>
       <c r="B113" s="13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C113" s="13"/>
       <c r="D113" s="13"/>
@@ -4368,7 +4371,7 @@
     <row r="114" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2"/>
       <c r="B114" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C114" s="13"/>
       <c r="D114" s="13"/>
@@ -4396,7 +4399,7 @@
     <row r="115" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2"/>
       <c r="B115" s="13" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C115" s="13"/>
       <c r="D115" s="13"/>
@@ -4424,7 +4427,7 @@
     <row r="116" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2"/>
       <c r="B116" s="13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C116" s="13"/>
       <c r="D116" s="13"/>
@@ -4452,7 +4455,7 @@
     <row r="117" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2"/>
       <c r="B117" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C117" s="13"/>
       <c r="D117" s="13"/>
@@ -4479,38 +4482,38 @@
     </row>
     <row r="118" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2"/>
-      <c r="B118" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="C118" s="20"/>
-      <c r="D118" s="20"/>
-      <c r="E118" s="20"/>
-      <c r="F118" s="20"/>
-      <c r="G118" s="20"/>
-      <c r="H118" s="20"/>
-      <c r="I118" s="20"/>
-      <c r="J118" s="20"/>
-      <c r="K118" s="20"/>
-      <c r="L118" s="20"/>
-      <c r="M118" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="N118" s="20"/>
-      <c r="O118" s="20"/>
-      <c r="P118" s="20"/>
-      <c r="Q118" s="20"/>
-      <c r="R118" s="20"/>
-      <c r="S118" s="20"/>
-      <c r="T118" s="20"/>
-      <c r="U118" s="20"/>
-      <c r="V118" s="20"/>
-      <c r="W118" s="20"/>
-      <c r="X118" s="20"/>
+      <c r="B118" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="C118" s="24"/>
+      <c r="D118" s="24"/>
+      <c r="E118" s="24"/>
+      <c r="F118" s="24"/>
+      <c r="G118" s="24"/>
+      <c r="H118" s="24"/>
+      <c r="I118" s="24"/>
+      <c r="J118" s="24"/>
+      <c r="K118" s="24"/>
+      <c r="L118" s="24"/>
+      <c r="M118" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="N118" s="24"/>
+      <c r="O118" s="24"/>
+      <c r="P118" s="24"/>
+      <c r="Q118" s="24"/>
+      <c r="R118" s="24"/>
+      <c r="S118" s="24"/>
+      <c r="T118" s="24"/>
+      <c r="U118" s="24"/>
+      <c r="V118" s="24"/>
+      <c r="W118" s="24"/>
+      <c r="X118" s="24"/>
     </row>
     <row r="119" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2"/>
       <c r="B119" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C119" s="9"/>
       <c r="D119" s="9"/>
@@ -4644,7 +4647,7 @@
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
       <c r="D124" s="13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E124" s="13"/>
       <c r="F124" s="13"/>
@@ -4657,7 +4660,7 @@
       <c r="M124" s="2"/>
       <c r="N124" s="2"/>
       <c r="O124" s="13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="P124" s="13"/>
       <c r="Q124" s="13"/>
@@ -4685,7 +4688,7 @@
       <c r="M125" s="2"/>
       <c r="N125" s="2"/>
       <c r="O125" s="13" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="P125" s="13"/>
       <c r="Q125" s="13"/>
@@ -4713,11 +4716,11 @@
       <c r="M126" s="2"/>
       <c r="N126" s="2"/>
       <c r="O126" s="13" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="P126" s="13"/>
       <c r="Q126" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R126" s="12"/>
       <c r="S126" s="12"/>
@@ -4742,7 +4745,7 @@
       <c r="M127" s="2"/>
       <c r="N127" s="2"/>
       <c r="O127" s="13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="P127" s="13"/>
       <c r="Q127" s="13"/>
@@ -4927,7 +4930,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="B23:X39 B68:X69 C67:X67 B71:X128 C70:X70 B41:X66 B40:F40 A39:A127 A1:A38 Y1:Y127 B1:X21" numberStoredAsText="1"/>
+    <ignoredError sqref="B23:X26 B68:X69 C67:X67 B71:X128 C70:X70 B41:X66 B40:F40 A39:A127 A1:A38 Y1:Y127 B1:X1 B3:X14 B2:D2 M2:X2 B16:X21 B15:C15 B28:X39" numberStoredAsText="1"/>
   </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>